<commit_message>
-Fixed an issue in Logging message when importing request --> exporting response. -ProfileExecutionIDEnum has been updated to 2.1.0 -ResponseTypeEnum updates: value ALPHA_INDICATOR changed to INDICATOR value ECONOMIC_OPERATOR_ROLE_CODE changed to CODE -ArtefactUtils now has a findDocumentDetails method -CODE_BOOLEAN mapped to ExpectedCode in XML artefact level
</commit_message>
<xml_diff>
--- a/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0.xlsx
+++ b/builder/src/main/resources/templates/v2_regulated/ESPD-CriteriaTaxonomy-REGULATED-V2.1.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ESPD-EDM\docs\src\main\asciidoc\dist\cl\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NetbeansProjects\espd-vcd-system\builder\src\main\resources\templates\v2_regulated\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEC4703-80EB-4E33-8B71-D53A0C0B1F97}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="588" firstSheet="30" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11493" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11493" uniqueCount="442">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1357,9 +1358,6 @@
     <t>CountryCodeIdentifier</t>
   </si>
   <si>
-    <t>ALPHA_INDICATOR</t>
-  </si>
-  <si>
     <t>Please indicate the role of the economic operator in the group (leader, responsible for specific tasks...)</t>
   </si>
   <si>
@@ -1390,7 +1388,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2350,52 +2348,80 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="42"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Έμφαση6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Έμφαση6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Έμφαση6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Εισαγωγή" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Έλεγχος κελιού" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Έμφαση1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Έμφαση2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Έμφαση3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Έμφαση4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Έμφαση5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Έμφαση6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Έξοδος" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Επεξηγηματικό κείμενο" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Επικεφαλίδα 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Κακό" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Καλό" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Ουδέτερο" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Προειδοποιητικό κείμενο" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Σημείωση" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Συνδεδεμένο κελί" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Σύνολο" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Τίτλος" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Υπολογισμός" xfId="11" builtinId="22" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{B7A466B9-B029-411E-89CF-A6B304918CC2}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2424,7 +2450,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectángulo 3"/>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2479,7 +2511,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectángulo 4"/>
+        <xdr:cNvPr id="5" name="Rectángulo 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2534,7 +2572,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Conector angular 11"/>
+        <xdr:cNvPr id="12" name="Conector angular 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="5" idx="0"/>
           <a:endCxn id="4" idx="3"/>
@@ -2584,7 +2628,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Rectángulo 12"/>
+        <xdr:cNvPr id="13" name="Rectángulo 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2639,7 +2689,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Rectángulo 13"/>
+        <xdr:cNvPr id="14" name="Rectángulo 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2694,7 +2750,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Conector angular 15"/>
+        <xdr:cNvPr id="16" name="Conector angular 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="13" idx="0"/>
           <a:endCxn id="14" idx="3"/>
@@ -2744,7 +2806,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Rectángulo 16"/>
+        <xdr:cNvPr id="17" name="Rectángulo 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2799,7 +2867,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Rectángulo 17"/>
+        <xdr:cNvPr id="18" name="Rectángulo 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2854,7 +2928,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="20" name="Conector angular 19"/>
+        <xdr:cNvPr id="20" name="Conector angular 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="17" idx="0"/>
           <a:endCxn id="18" idx="3"/>
@@ -2904,7 +2984,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Rectángulo 20"/>
+        <xdr:cNvPr id="21" name="Rectángulo 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2959,7 +3045,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="Conector angular 22"/>
+        <xdr:cNvPr id="23" name="Conector angular 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="21" idx="3"/>
           <a:endCxn id="18" idx="3"/>
@@ -3011,7 +3103,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="Rectángulo 24"/>
+        <xdr:cNvPr id="25" name="Rectángulo 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3066,7 +3164,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Rectángulo 25"/>
+        <xdr:cNvPr id="26" name="Rectángulo 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3121,7 +3225,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="28" name="Conector angular 27"/>
+        <xdr:cNvPr id="28" name="Conector angular 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="25" idx="0"/>
           <a:endCxn id="26" idx="3"/>
@@ -3171,7 +3281,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="Rectángulo 28"/>
+        <xdr:cNvPr id="29" name="Rectángulo 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3226,7 +3342,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="Rectángulo 29"/>
+        <xdr:cNvPr id="30" name="Rectángulo 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3281,7 +3403,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Conector angular 30"/>
+        <xdr:cNvPr id="31" name="Conector angular 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="29" idx="0"/>
           <a:endCxn id="30" idx="3"/>
@@ -3331,7 +3459,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="Rectángulo 31"/>
+        <xdr:cNvPr id="32" name="Rectángulo 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000020000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3386,7 +3520,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="Rectángulo 32"/>
+        <xdr:cNvPr id="33" name="Rectángulo 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3441,7 +3581,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="34" name="Conector angular 33"/>
+        <xdr:cNvPr id="34" name="Conector angular 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="33" idx="0"/>
           <a:endCxn id="32" idx="3"/>
@@ -3491,7 +3637,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="Rectángulo 34"/>
+        <xdr:cNvPr id="35" name="Rectángulo 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3546,7 +3698,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="Rectángulo 35"/>
+        <xdr:cNvPr id="36" name="Rectángulo 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3601,7 +3759,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="37" name="Conector angular 36"/>
+        <xdr:cNvPr id="37" name="Conector angular 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="35" idx="0"/>
           <a:endCxn id="36" idx="3"/>
@@ -3651,7 +3815,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="Rectángulo 37"/>
+        <xdr:cNvPr id="38" name="Rectángulo 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000026000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3706,7 +3876,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="Rectángulo 38"/>
+        <xdr:cNvPr id="39" name="Rectángulo 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3761,7 +3937,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="40" name="Conector angular 39"/>
+        <xdr:cNvPr id="40" name="Conector angular 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="38" idx="0"/>
           <a:endCxn id="39" idx="3"/>
@@ -3811,7 +3993,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="Rectángulo 40"/>
+        <xdr:cNvPr id="41" name="Rectángulo 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3866,7 +4054,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="42" name="Conector angular 41"/>
+        <xdr:cNvPr id="42" name="Conector angular 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="41" idx="3"/>
           <a:endCxn id="39" idx="3"/>
@@ -3918,7 +4112,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="Rectángulo 42"/>
+        <xdr:cNvPr id="43" name="Rectángulo 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -3973,7 +4173,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name="Rectángulo 43"/>
+        <xdr:cNvPr id="44" name="Rectángulo 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4028,7 +4234,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="45" name="Conector angular 44"/>
+        <xdr:cNvPr id="45" name="Conector angular 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="43" idx="0"/>
           <a:endCxn id="44" idx="3"/>
@@ -4078,7 +4290,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="Rectángulo 45"/>
+        <xdr:cNvPr id="46" name="Rectángulo 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4133,7 +4351,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="Rectángulo 46"/>
+        <xdr:cNvPr id="47" name="Rectángulo 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -4188,7 +4412,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="48" name="Conector angular 47"/>
+        <xdr:cNvPr id="48" name="Conector angular 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="46" idx="0"/>
           <a:endCxn id="47" idx="3"/>
@@ -4227,7 +4457,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4302,6 +4532,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -4337,6 +4584,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4512,13 +4776,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:Z146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="55" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="10.7109375" style="25" customWidth="1"/>
@@ -12028,12 +12292,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T23" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T47" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T71" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T95" r:id="rId4" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T119" r:id="rId5" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T143" r:id="rId6" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T23" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="T47" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="T71" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="T95" r:id="rId4" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="T119" r:id="rId5" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="T143" r:id="rId6" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId7"/>
@@ -12041,13 +12305,13 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Hoja10"/>
   <dimension ref="A1:AX26"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="2" customWidth="1"/>
@@ -13447,8 +13711,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T23" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="T23" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId3"/>
@@ -13456,13 +13720,13 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Hoja11"/>
   <dimension ref="A1:AX32"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -15346,15 +15610,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T29" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="T29" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Hoja12"/>
   <dimension ref="A1:Z15"/>
   <sheetViews>
@@ -15362,7 +15626,7 @@
       <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="68" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="66" bestFit="1" customWidth="1"/>
@@ -16178,7 +16442,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T12" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T12" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -16186,13 +16450,13 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Hoja13"/>
   <dimension ref="A1:AX15"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -17029,20 +17293,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T12" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T12" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Hoja14"/>
   <dimension ref="A1:AX15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="7" customWidth="1"/>
@@ -17862,20 +18126,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T12" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T12" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Hoja15"/>
   <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -18192,7 +18456,7 @@
       </c>
       <c r="Y5" s="20"/>
       <c r="Z5" s="133" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="66" customFormat="1" x14ac:dyDescent="0.25">
@@ -18709,7 +18973,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T12" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T12" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -18717,13 +18981,13 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Hoja16"/>
   <dimension ref="A1:AX14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="57" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="54" bestFit="1" customWidth="1"/>
@@ -19633,7 +19897,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -19641,13 +19905,13 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Hoja17"/>
   <dimension ref="A1:AX15"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="80" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="15" customWidth="1"/>
@@ -20553,7 +20817,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T12" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T12" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId2"/>
@@ -20561,13 +20825,13 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Hoja18"/>
   <dimension ref="A1:AX14"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="57" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" style="54" customWidth="1"/>
@@ -21470,7 +21734,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -21478,7 +21742,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr codeName="Hoja19"/>
   <dimension ref="A1:AX14"/>
   <sheetViews>
@@ -21486,7 +21750,7 @@
       <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="57" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" style="54" customWidth="1"/>
@@ -22379,14 +22643,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -22394,7 +22658,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="10.7109375" style="15" customWidth="1"/>
@@ -25870,8 +26134,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T34" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T69" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T34" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="T69" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId3"/>
@@ -25880,13 +26144,13 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Hoja20"/>
   <dimension ref="A1:Z48"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.7109375" style="25" customWidth="1"/>
@@ -28303,9 +28567,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T29" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T44" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="T29" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
+    <hyperlink ref="T44" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId4"/>
@@ -28313,13 +28577,13 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Hoja21"/>
   <dimension ref="A1:Z98"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.7109375" style="10" customWidth="1"/>
@@ -33197,27 +33461,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T23" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T35" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T47" r:id="rId4" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T59" r:id="rId5" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T71" r:id="rId6" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T83" r:id="rId7" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T95" r:id="rId8" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="T23" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
+    <hyperlink ref="T35" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1400-000002000000}"/>
+    <hyperlink ref="T47" r:id="rId4" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1400-000003000000}"/>
+    <hyperlink ref="T59" r:id="rId5" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1400-000004000000}"/>
+    <hyperlink ref="T71" r:id="rId6" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1400-000005000000}"/>
+    <hyperlink ref="T83" r:id="rId7" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1400-000006000000}"/>
+    <hyperlink ref="T95" r:id="rId8" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1400-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Hoja22"/>
   <dimension ref="A1:AX14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" style="10" customWidth="1"/>
@@ -33996,20 +34260,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr codeName="Hoja23"/>
   <dimension ref="A1:AX44"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="10" customWidth="1"/>
@@ -36219,21 +36483,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T20" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T41" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T20" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
+    <hyperlink ref="T41" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr codeName="Hoja24"/>
   <dimension ref="A1:AX14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -37123,14 +37387,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr codeName="Hoja25"/>
   <dimension ref="A1:AX26"/>
   <sheetViews>
@@ -37138,7 +37402,7 @@
       <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="10" customWidth="1"/>
@@ -38526,15 +38790,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T23" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
+    <hyperlink ref="T23" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1800-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr codeName="Hoja26"/>
   <dimension ref="A1:AX47"/>
   <sheetViews>
@@ -38542,7 +38806,7 @@
       <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
@@ -41127,9 +41391,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T29" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T44" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
+    <hyperlink ref="T29" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1900-000001000000}"/>
+    <hyperlink ref="T44" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1900-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId4"/>
@@ -41137,13 +41401,13 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr codeName="Hoja27"/>
   <dimension ref="A1:AX141"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
@@ -42716,20 +42980,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <sheetPr codeName="Hoja28"/>
   <dimension ref="A1:AX149"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="38" customWidth="1"/>
@@ -44892,20 +45156,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T22" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T22" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <sheetPr codeName="Hoja29"/>
   <dimension ref="A1:AX142"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
@@ -45380,7 +45644,7 @@
       <c r="Q7" s="34"/>
       <c r="R7" s="96"/>
       <c r="S7" s="28" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="T7" s="28" t="s">
         <v>372</v>
@@ -45389,13 +45653,13 @@
         <v>1</v>
       </c>
       <c r="V7" s="145" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="W7" s="100"/>
       <c r="X7" s="101"/>
       <c r="Y7" s="101"/>
       <c r="Z7" s="147" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AA7"/>
       <c r="AB7"/>
@@ -45450,7 +45714,7 @@
       <c r="Q8" s="34"/>
       <c r="R8" s="96"/>
       <c r="S8" s="28" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="T8" s="28" t="s">
         <v>372</v>
@@ -45516,7 +45780,7 @@
       <c r="Q9" s="34"/>
       <c r="R9" s="96"/>
       <c r="S9" s="28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="T9" s="28" t="s">
         <v>372</v>
@@ -46657,20 +46921,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T15" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T15" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:AX65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" style="25" bestFit="1" customWidth="1"/>
@@ -51197,9 +51461,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T20" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T41" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T62" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T20" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="T41" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="T62" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -51207,13 +51471,13 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <sheetPr codeName="Hoja30"/>
   <dimension ref="A1:Z38"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
@@ -52476,14 +52740,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T15" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T15" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <sheetPr codeName="Hoja31"/>
   <dimension ref="A1:AX18"/>
   <sheetViews>
@@ -52491,7 +52755,7 @@
       <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
@@ -53585,20 +53849,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T15" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T15" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <sheetPr codeName="Hoja32"/>
   <dimension ref="A1:AX137"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" style="39" customWidth="1"/>
@@ -55001,14 +55265,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T10" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T10" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <sheetPr codeName="Hoja33"/>
   <dimension ref="A1:AX137"/>
   <sheetViews>
@@ -55016,7 +55280,7 @@
       <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="39" customWidth="1"/>
@@ -56305,14 +56569,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T10" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T10" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <sheetPr codeName="Hoja34"/>
   <dimension ref="A1:AX17"/>
   <sheetViews>
@@ -56320,7 +56584,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="16" width="0" hidden="1" customWidth="1"/>
@@ -56508,7 +56772,7 @@
       <c r="U3" s="95"/>
       <c r="V3" s="31"/>
       <c r="W3" s="98" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="X3" s="98" t="s">
         <v>430</v>
@@ -57325,7 +57589,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -57333,15 +57597,15 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <sheetPr codeName="Hoja35"/>
   <dimension ref="A1:AX13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="7" max="16" width="0" hidden="1" customWidth="1"/>
@@ -57528,7 +57792,7 @@
       <c r="U3" s="95"/>
       <c r="V3" s="31"/>
       <c r="W3" s="98" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="X3" s="98" t="s">
         <v>429</v>
@@ -57673,7 +57937,7 @@
         <v>1</v>
       </c>
       <c r="V5" s="145" t="s">
-        <v>433</v>
+        <v>17</v>
       </c>
       <c r="W5" s="100"/>
       <c r="X5" s="101" t="s">
@@ -57681,7 +57945,7 @@
       </c>
       <c r="Y5" s="101"/>
       <c r="Z5" s="145" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AA5" s="111"/>
       <c r="AB5" s="111"/>
@@ -58120,20 +58384,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T10" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T10" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:AX98"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.7109375" style="7" customWidth="1"/>
@@ -63461,25 +63725,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T15" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T31" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T47" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T63" r:id="rId4" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T79" r:id="rId5" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T95" r:id="rId6" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T15" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="T31" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="T47" r:id="rId3" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="T63" r:id="rId4" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="T79" r:id="rId5" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="T95" r:id="rId6" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:AX44"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="10.7109375" customWidth="1"/>
@@ -66335,8 +66599,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T20" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T41" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T20" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="T41" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -66344,13 +66608,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:AX34"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.7109375" customWidth="1"/>
@@ -68381,8 +68645,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
-    <hyperlink ref="T29" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T14" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="T29" r:id="rId2" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -68390,13 +68654,13 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:AX23"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="10.7109375" style="2" customWidth="1"/>
@@ -69636,20 +69900,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T20" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T20" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="42" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.7109375" style="38" customWidth="1"/>
@@ -70388,7 +70652,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T11" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -70396,13 +70660,13 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:AX23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="56" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="10.7109375" style="56" customWidth="1"/>
@@ -71709,7 +71973,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="T20" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001"/>
+    <hyperlink ref="T20" r:id="rId1" display="http://public_site/repository/evidences/evidence?id=EVIDENCE-00001" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>